<commit_message>
performance report new API's added
</commit_message>
<xml_diff>
--- a/Output Data/Crpo/Common_folder/Performance/chart_analysis.xlsx
+++ b/Output Data/Crpo/Common_folder/Performance/chart_analysis.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>get_tenant_details</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t>getTestUsersForTest</t>
+  </si>
+  <si>
+    <t>interview</t>
+  </si>
+  <si>
+    <t>interview_new</t>
   </si>
   <si>
     <t>AMSIN_NON_EU</t>
@@ -170,16 +176,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.21832058095238</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.497181979365079</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.086442057142857</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.87266203968254</c:v>
+                  <c:v>1.161827581294963</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.448821469064748</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.021376739568345</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.839213437410072</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -233,16 +239,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.9935309603174607</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.27542769047619</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.368625688888889</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.128819355555556</c:v>
+                  <c:v>0.9352611208633096</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.202469553956834</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.284911778417266</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.056331359712231</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -296,16 +302,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.046826265079365</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.730245468253969</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.386791787301588</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.99613370952381</c:v>
+                  <c:v>0.984325598561151</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.661092615827339</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.323073283453238</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.939246870503598</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -359,16 +365,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.617602347619048</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.322371144444445</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.922480903174604</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.765872276190475</c:v>
+                  <c:v>1.57429501294964</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.282897650359712</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.859480120863311</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.716341187050359</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -422,16 +428,142 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.9433901285714285</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.7193199</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.232480744444445</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.781353692063492</c:v>
+                  <c:v>0.8922638676258993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.64759233381295</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.168918392805756</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.710564005755395</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Dashboard!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>interview</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Dashboard!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>AMSIN_NON_EU</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AMSIN_EU</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>LIVE_NON_EU</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>LIVE_EU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Dashboard!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.1159046748201439</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.06540645179856117</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.07801122158273381</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.07795220863309353</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Dashboard!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>interview_new</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Dashboard!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>AMSIN_NON_EU</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AMSIN_EU</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>LIVE_NON_EU</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>LIVE_EU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Dashboard!$H$2:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.05025791366906475</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.04741873956834533</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.03567814244604316</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.06213537122302158</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -837,13 +969,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -859,85 +991,115 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>1.21832058095238</v>
+        <v>1.161827581294963</v>
       </c>
       <c r="C2">
-        <v>0.9935309603174607</v>
+        <v>0.9352611208633096</v>
       </c>
       <c r="D2">
-        <v>1.046826265079365</v>
+        <v>0.984325598561151</v>
       </c>
       <c r="E2">
-        <v>1.617602347619048</v>
+        <v>1.57429501294964</v>
       </c>
       <c r="F2">
-        <v>0.9433901285714285</v>
+        <v>0.8922638676258993</v>
+      </c>
+      <c r="G2">
+        <v>0.1159046748201439</v>
+      </c>
+      <c r="H2">
+        <v>0.05025791366906475</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>2.497181979365079</v>
+        <v>2.448821469064748</v>
       </c>
       <c r="C3">
-        <v>2.27542769047619</v>
+        <v>2.202469553956834</v>
       </c>
       <c r="D3">
-        <v>1.730245468253969</v>
+        <v>1.661092615827339</v>
       </c>
       <c r="E3">
-        <v>2.322371144444445</v>
+        <v>2.282897650359712</v>
       </c>
       <c r="F3">
-        <v>1.7193199</v>
+        <v>1.64759233381295</v>
+      </c>
+      <c r="G3">
+        <v>0.06540645179856117</v>
+      </c>
+      <c r="H3">
+        <v>0.04741873956834533</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>1.086442057142857</v>
+        <v>1.021376739568345</v>
       </c>
       <c r="C4">
-        <v>1.368625688888889</v>
+        <v>1.284911778417266</v>
       </c>
       <c r="D4">
-        <v>1.386791787301588</v>
+        <v>1.323073283453238</v>
       </c>
       <c r="E4">
-        <v>1.922480903174604</v>
+        <v>1.859480120863311</v>
       </c>
       <c r="F4">
-        <v>1.232480744444445</v>
+        <v>1.168918392805756</v>
+      </c>
+      <c r="G4">
+        <v>0.07801122158273381</v>
+      </c>
+      <c r="H4">
+        <v>0.03567814244604316</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>3.87266203968254</v>
+        <v>3.839213437410072</v>
       </c>
       <c r="C5">
-        <v>2.128819355555556</v>
+        <v>2.056331359712231</v>
       </c>
       <c r="D5">
-        <v>1.99613370952381</v>
+        <v>1.939246870503598</v>
       </c>
       <c r="E5">
-        <v>2.765872276190475</v>
+        <v>2.716341187050359</v>
       </c>
       <c r="F5">
-        <v>1.781353692063492</v>
+        <v>1.710564005755395</v>
+      </c>
+      <c r="G5">
+        <v>0.07795220863309353</v>
+      </c>
+      <c r="H5">
+        <v>0.06213537122302158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New changes in test suite support
</commit_message>
<xml_diff>
--- a/Output Data/Crpo/Common_folder/Performance/chart_analysis.xlsx
+++ b/Output Data/Crpo/Common_folder/Performance/chart_analysis.xlsx
@@ -170,16 +170,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.7992404388206373</c:v>
+                  <c:v>0.79263823653846</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.950409954791151</c:v>
+                  <c:v>1.928472638942304</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7637763631449633</c:v>
+                  <c:v>0.7579752721153847</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.49143926191646</c:v>
+                  <c:v>2.464334802403844</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -233,16 +233,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.7103929941031946</c:v>
+                  <c:v>0.705740642307693</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.115030205896804</c:v>
+                  <c:v>2.100594170192307</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9524272437346444</c:v>
+                  <c:v>0.9449168495192313</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.903671383292383</c:v>
+                  <c:v>1.899966336538461</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -296,16 +296,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.7187199361179355</c:v>
+                  <c:v>0.7128991173076918</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.730219414742014</c:v>
+                  <c:v>1.717727036057692</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9749997936117935</c:v>
+                  <c:v>0.9685790293269226</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.61300626977887</c:v>
+                  <c:v>1.607334240384615</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -359,16 +359,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.527647508599508</c:v>
+                  <c:v>1.51125994326923</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.401903486240788</c:v>
+                  <c:v>2.385732178125001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.321636717936119</c:v>
+                  <c:v>1.310371479807694</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.635120054054054</c:v>
+                  <c:v>2.646548055769231</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -422,16 +422,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.7201862466830461</c:v>
+                  <c:v>0.7189450956730764</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.738080533169533</c:v>
+                  <c:v>1.727314515865384</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9195452343980349</c:v>
+                  <c:v>0.9139563562500003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.578963326289927</c:v>
+                  <c:v>1.577224537500001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -865,19 +865,19 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0.7992404388206373</v>
+        <v>0.79263823653846</v>
       </c>
       <c r="C2">
-        <v>0.7103929941031946</v>
+        <v>0.705740642307693</v>
       </c>
       <c r="D2">
-        <v>0.7187199361179355</v>
+        <v>0.7128991173076918</v>
       </c>
       <c r="E2">
-        <v>1.527647508599508</v>
+        <v>1.51125994326923</v>
       </c>
       <c r="F2">
-        <v>0.7201862466830461</v>
+        <v>0.7189450956730764</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -885,19 +885,19 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>1.950409954791151</v>
+        <v>1.928472638942304</v>
       </c>
       <c r="C3">
-        <v>2.115030205896804</v>
+        <v>2.100594170192307</v>
       </c>
       <c r="D3">
-        <v>1.730219414742014</v>
+        <v>1.717727036057692</v>
       </c>
       <c r="E3">
-        <v>2.401903486240788</v>
+        <v>2.385732178125001</v>
       </c>
       <c r="F3">
-        <v>1.738080533169533</v>
+        <v>1.727314515865384</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -905,19 +905,19 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0.7637763631449633</v>
+        <v>0.7579752721153847</v>
       </c>
       <c r="C4">
-        <v>0.9524272437346444</v>
+        <v>0.9449168495192313</v>
       </c>
       <c r="D4">
-        <v>0.9749997936117935</v>
+        <v>0.9685790293269226</v>
       </c>
       <c r="E4">
-        <v>1.321636717936119</v>
+        <v>1.310371479807694</v>
       </c>
       <c r="F4">
-        <v>0.9195452343980349</v>
+        <v>0.9139563562500003</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -925,19 +925,19 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>2.49143926191646</v>
+        <v>2.464334802403844</v>
       </c>
       <c r="C5">
-        <v>1.903671383292383</v>
+        <v>1.899966336538461</v>
       </c>
       <c r="D5">
-        <v>1.61300626977887</v>
+        <v>1.607334240384615</v>
       </c>
       <c r="E5">
-        <v>2.635120054054054</v>
+        <v>2.646548055769231</v>
       </c>
       <c r="F5">
-        <v>1.578963326289927</v>
+        <v>1.577224537500001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>